<commit_message>
220525 : 0627 commit
</commit_message>
<xml_diff>
--- a/쿼리문서.xlsx
+++ b/쿼리문서.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{74C9E52F-23EC-4A5C-93B6-C1786BBF2B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{13EA097F-9180-4E12-B650-FD28BCD85384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{116C8692-C26E-4F46-AA31-39B894195CC1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{116C8692-C26E-4F46-AA31-39B894195CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -128,42 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT CHAT_ID, ROOM_ID, EMP_ID, CHAT_CON,CHAT_TIME,CHAT_TYPE
-    FROM CHAT 
-        WHERE ROOM_ID = '4'  
-        AND CHAT_TIME &gt;= (
-                SELECT TO_DATE(jt.JDATE,'YYYYMMDDHH24MISS')
-                    FROM CHAT_ROOM,
-                    JSON_TABLE(ROOM_MEM, '$.ROOM[*]'
-                        COLUMNS (
-                            IDS VARCHAR(20) PATH '$.id',
-                            JDATE VARCHAR(30) PATH '$.join'
-                        )
-                    ) AS jt
-                    WHERE IDS = '5' AND ROOM_ID = '4'
-        )
-        ORDER BY TO_NUMBER(CHAT_ID);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT cr.ROOM_ID, cr.ROOM_NAME, CHAT_TIME, CHAT_ID, EMP_ID
-    FROM CHAT_ROOM cr,
-        JSON_TABLE(ROOM_MEM, '$.ROOM[*]'
-            COLUMNS (
-                IDS VARCHAR(20) PATH '$.id'
-            )
-        ) AS jt,
-        (SELECT ROOM_ID, EMP_ID ,CHAT_ID ,CHAT_TIME ,
-                   ROW_NUMBER () OVER(PARTITION BY ROOM_ID ORDER BY CHAT_TIME DESC) AS mx
-            FROM CHAT
-        ) ch
-    WHERE IDS = '5'
-    AND cr.ROOM_ID = ch.ROOM_ID
-    AND mx = 1
-    ORDER BY CHAT_ID;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insFile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -191,6 +147,43 @@
   </si>
   <si>
     <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT ch.ROOM_ID, ROOM_NAME, CHAT_TIME, CHAT_ID, CHAT_TYPE ,EMP_ID,CHAT_CON
+    		FROM CHAT_ROOM cr,
+	        	JSON_TABLE(ROOM_MEM, '$.ROOM[*]'
+	            	COLUMNS (
+	                	IDS VARCHAR(20) PATH '$.id'
+	            	)
+	        	) AS jt,
+	        	(SELECT ROOM_ID, EMP_ID ,CHAT_ID ,
+	        			CHAT_TIME , CHAT_TYPE, CHAT_CON,
+	                    ROW_NUMBER () OVER(PARTITION BY ROOM_ID ORDER BY CHAT_TIME DESC) AS mx
+	            	FROM CHAT
+	        	) ch
+    		WHERE IDS = '2022052800'
+    		AND cr.ROOM_ID = ch.ROOM_ID
+    		AND mx = 1
+    		ORDER BY CHAT_ID;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT CHAT_ID, EMP_ID, CHAT_CON, CHAT_TIME, CHAT_TYPE
+	FROM CHAT 
+	WHERE ROOM_ID = '4'  
+	AND CHAT_TIME &gt;= (
+		SELECT TO_DATE(jt.JDATE,'YYYYMMDDHH24MISS')
+			FROM CHAT_ROOM,
+			JSON_TABLE(ROOM_MEM, '$.ROOM[*]'
+				COLUMNS (
+		 			IDS VARCHAR(20) PATH '$.id',
+		 			JDATE VARCHAR(30) PATH '$.join'
+				)
+			) AS jt
+			WHERE IDS = '2022052800' AND ROOM_ID = '4'
+	)
+	ORDER BY TO_NUMBER(CHAT_ID);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -566,19 +559,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A03F8B7B-D6A8-4983-B107-CE0ACA7924F0}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="95.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="247.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="272" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -603,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -612,7 +605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="247.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -620,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -629,7 +622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -640,15 +633,15 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -657,13 +650,13 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -674,13 +667,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="132" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="136" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -691,18 +684,18 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>